<commit_message>
Prepared Docs for Sphinx
</commit_message>
<xml_diff>
--- a/XlsxWriterExample.xlsx
+++ b/XlsxWriterExample.xlsx
@@ -502,34 +502,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -592,34 +592,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1177,10 +1177,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1188,10 +1188,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1199,10 +1199,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1213,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1221,10 +1221,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1232,10 +1232,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1243,7 +1243,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1254,10 +1254,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1265,10 +1265,10 @@
         <v>8</v>
       </c>
       <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
         <v>5</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1276,10 +1276,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>